<commit_message>
+ My new resource to avoid broken image in Galaxy Y
</commit_message>
<xml_diff>
--- a/trunk/TEMP/level.xlsx
+++ b/trunk/TEMP/level.xlsx
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EB148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X37" sqref="X34:X37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
+ New Menuscene resource + Level design in high score
</commit_message>
<xml_diff>
--- a/trunk/TEMP/level.xlsx
+++ b/trunk/TEMP/level.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="15345" windowHeight="4755"/>
+    <workbookView xWindow="0" yWindow="4950" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="level" sheetId="1" r:id="rId1"/>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EB148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2253,7 @@
         <v>3</v>
       </c>
       <c r="S16">
-        <f t="shared" ref="Q16:S46" si="11">R16-1</f>
+        <f t="shared" ref="Q16:S30" si="11">R16-1</f>
         <v>2</v>
       </c>
       <c r="T16">
@@ -5351,7 +5351,7 @@
         <v>0.16</v>
       </c>
       <c r="I57">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J57" s="3">
         <v>0</v>
@@ -5434,7 +5434,7 @@
         <v>0.16</v>
       </c>
       <c r="I58">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J58" s="3">
         <v>0</v>
@@ -5510,7 +5510,7 @@
         <v>0.16</v>
       </c>
       <c r="I59">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J59" s="3">
         <v>0</v>
@@ -5586,7 +5586,7 @@
         <v>0.16</v>
       </c>
       <c r="I60">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J60" s="3">
         <v>0</v>
@@ -5662,7 +5662,7 @@
         <v>0.16</v>
       </c>
       <c r="I61">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J61" s="3">
         <v>0</v>
@@ -5738,7 +5738,7 @@
         <v>0.16</v>
       </c>
       <c r="I62">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J62" s="3">
         <v>0</v>
@@ -5814,7 +5814,7 @@
         <v>0.16</v>
       </c>
       <c r="I63">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J63" s="3">
         <v>0</v>
@@ -5890,7 +5890,7 @@
         <v>0.16</v>
       </c>
       <c r="I64">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J64" s="3">
         <v>0</v>
@@ -5966,7 +5966,7 @@
         <v>0.16</v>
       </c>
       <c r="I65">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J65" s="3">
         <v>0</v>
@@ -6042,7 +6042,7 @@
         <v>0.16</v>
       </c>
       <c r="I66">
-        <v>0.22500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J66" s="3">
         <v>0</v>
@@ -6118,7 +6118,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I67">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J67" s="3">
         <v>0</v>
@@ -6201,7 +6201,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I68">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J68" s="3">
         <v>0</v>
@@ -6277,7 +6277,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I69">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J69" s="3">
         <v>0</v>
@@ -6353,7 +6353,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I70">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J70" s="3">
         <v>0</v>
@@ -6429,7 +6429,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I71">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J71" s="3">
         <v>0</v>
@@ -6505,7 +6505,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I72">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J72" s="3">
         <v>0</v>
@@ -6581,7 +6581,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I73">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J73" s="3">
         <v>0</v>
@@ -6657,7 +6657,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I74">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J74" s="3">
         <v>0</v>
@@ -6733,7 +6733,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I75">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J75" s="3">
         <v>0</v>
@@ -6809,7 +6809,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I76">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J76" s="3">
         <v>0</v>
@@ -6885,7 +6885,7 @@
         <v>0.12</v>
       </c>
       <c r="I77">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J77" s="3">
         <v>0</v>
@@ -6932,7 +6932,7 @@
         <v>2</v>
       </c>
       <c r="X77">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z77"/>
       <c r="AA77"/>
@@ -6968,7 +6968,7 @@
         <v>0.12</v>
       </c>
       <c r="I78">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J78" s="3">
         <v>0</v>
@@ -6987,7 +6987,7 @@
         <v>33</v>
       </c>
       <c r="O78">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="P78" s="3">
         <v>0</v>
@@ -7015,7 +7015,7 @@
         <v>2</v>
       </c>
       <c r="X78">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:132" x14ac:dyDescent="0.25">
@@ -7044,7 +7044,7 @@
         <v>0.12</v>
       </c>
       <c r="I79">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J79" s="3">
         <v>0</v>
@@ -7063,7 +7063,7 @@
         <v>33</v>
       </c>
       <c r="O79">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P79" s="3">
         <v>0</v>
@@ -7091,7 +7091,7 @@
         <v>2</v>
       </c>
       <c r="X79">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:132" x14ac:dyDescent="0.25">
@@ -7120,7 +7120,7 @@
         <v>0.12</v>
       </c>
       <c r="I80">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J80" s="3">
         <v>0</v>
@@ -7139,7 +7139,7 @@
         <v>33</v>
       </c>
       <c r="O80">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="P80" s="3">
         <v>0</v>
@@ -7167,7 +7167,7 @@
         <v>2</v>
       </c>
       <c r="X80">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:132" x14ac:dyDescent="0.25">
@@ -7196,7 +7196,7 @@
         <v>0.12</v>
       </c>
       <c r="I81">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J81" s="3">
         <v>0</v>
@@ -7215,7 +7215,7 @@
         <v>35</v>
       </c>
       <c r="O81">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="P81" s="3">
         <v>0</v>
@@ -7243,7 +7243,7 @@
         <v>2</v>
       </c>
       <c r="X81">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:132" x14ac:dyDescent="0.25">
@@ -7272,7 +7272,7 @@
         <v>0.12</v>
       </c>
       <c r="I82">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J82" s="3">
         <v>0</v>
@@ -7291,7 +7291,7 @@
         <v>35</v>
       </c>
       <c r="O82">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="P82" s="3">
         <v>0</v>
@@ -7319,7 +7319,7 @@
         <v>2</v>
       </c>
       <c r="X82">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:132" x14ac:dyDescent="0.25">
@@ -7348,7 +7348,7 @@
         <v>0.12</v>
       </c>
       <c r="I83">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J83" s="3">
         <v>0</v>
@@ -7367,7 +7367,7 @@
         <v>35</v>
       </c>
       <c r="O83">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="P83" s="3">
         <v>0</v>
@@ -7395,7 +7395,7 @@
         <v>2</v>
       </c>
       <c r="X83">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:132" x14ac:dyDescent="0.25">
@@ -7424,7 +7424,7 @@
         <v>0.12</v>
       </c>
       <c r="I84">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J84" s="3">
         <v>0</v>
@@ -7440,10 +7440,10 @@
         <v>18</v>
       </c>
       <c r="N84" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O84">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="P84" s="3">
         <v>0</v>
@@ -7471,7 +7471,7 @@
         <v>2</v>
       </c>
       <c r="X84">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:132" x14ac:dyDescent="0.25">
@@ -7500,7 +7500,7 @@
         <v>0.12</v>
       </c>
       <c r="I85">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J85" s="3">
         <v>0</v>
@@ -7516,10 +7516,10 @@
         <v>18</v>
       </c>
       <c r="N85" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O85">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="P85" s="3">
         <v>0</v>
@@ -7547,7 +7547,7 @@
         <v>2</v>
       </c>
       <c r="X85">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:132" x14ac:dyDescent="0.25">
@@ -7576,7 +7576,7 @@
         <v>0.12</v>
       </c>
       <c r="I86">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J86" s="3">
         <v>0</v>
@@ -7592,10 +7592,10 @@
         <v>18</v>
       </c>
       <c r="N86" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O86">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="P86" s="3">
         <v>0</v>
@@ -7623,7 +7623,7 @@
         <v>2</v>
       </c>
       <c r="X86">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:132" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7652,7 +7652,7 @@
         <v>0.1</v>
       </c>
       <c r="I87">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J87" s="3">
         <v>0</v>
@@ -7668,10 +7668,10 @@
         <v>18</v>
       </c>
       <c r="N87" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="O87">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="P87" s="3">
         <v>0</v>
@@ -7735,7 +7735,7 @@
         <v>0.1</v>
       </c>
       <c r="I88">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J88" s="3">
         <v>0</v>
@@ -7751,10 +7751,10 @@
         <v>18</v>
       </c>
       <c r="N88" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="O88">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="P88" s="3">
         <v>0</v>
@@ -7811,7 +7811,7 @@
         <v>0.1</v>
       </c>
       <c r="I89">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J89" s="3">
         <v>0</v>
@@ -7827,10 +7827,10 @@
         <v>18</v>
       </c>
       <c r="N89" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="O89">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="P89" s="3">
         <v>0</v>
@@ -7887,7 +7887,7 @@
         <v>0.1</v>
       </c>
       <c r="I90">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J90" s="3">
         <v>0</v>
@@ -7903,10 +7903,10 @@
         <v>18</v>
       </c>
       <c r="N90" s="7">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="O90">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="P90" s="3">
         <v>0</v>
@@ -7963,7 +7963,7 @@
         <v>0.1</v>
       </c>
       <c r="I91">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J91" s="3">
         <v>0</v>
@@ -7979,10 +7979,10 @@
         <v>18</v>
       </c>
       <c r="N91" s="7">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="O91">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="P91" s="3">
         <v>0</v>
@@ -8039,7 +8039,7 @@
         <v>0.1</v>
       </c>
       <c r="I92">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J92" s="3">
         <v>0</v>
@@ -8055,10 +8055,10 @@
         <v>18</v>
       </c>
       <c r="N92" s="7">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="O92">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="P92" s="3">
         <v>0</v>
@@ -8115,7 +8115,7 @@
         <v>0.1</v>
       </c>
       <c r="I93">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J93" s="3">
         <v>0</v>
@@ -8131,10 +8131,10 @@
         <v>18</v>
       </c>
       <c r="N93" s="7">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="O93">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="P93" s="3">
         <v>0</v>
@@ -8191,7 +8191,7 @@
         <v>0.1</v>
       </c>
       <c r="I94">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J94" s="3">
         <v>0</v>
@@ -8207,10 +8207,10 @@
         <v>18</v>
       </c>
       <c r="N94" s="7">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="O94">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="P94" s="3">
         <v>0</v>
@@ -8267,7 +8267,7 @@
         <v>0.1</v>
       </c>
       <c r="I95">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J95" s="3">
         <v>0</v>
@@ -8283,10 +8283,10 @@
         <v>18</v>
       </c>
       <c r="N95" s="7">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="O95">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="P95" s="3">
         <v>0</v>
@@ -8343,7 +8343,7 @@
         <v>0.1</v>
       </c>
       <c r="I96">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J96" s="3">
         <v>0</v>
@@ -8359,10 +8359,10 @@
         <v>18</v>
       </c>
       <c r="N96" s="7">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="O96">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="P96" s="3">
         <v>0</v>
@@ -8419,7 +8419,7 @@
         <v>0.1</v>
       </c>
       <c r="I97">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="J97" s="3">
         <v>0</v>
@@ -8435,10 +8435,10 @@
         <v>18</v>
       </c>
       <c r="N97" s="7">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="O97">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="P97" s="3">
         <v>0</v>
@@ -8502,7 +8502,7 @@
         <v>0.1</v>
       </c>
       <c r="I98">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="J98" s="3">
         <v>0</v>
@@ -8518,10 +8518,10 @@
         <v>18</v>
       </c>
       <c r="N98" s="7">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="O98">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="P98" s="3">
         <v>0</v>
@@ -8578,7 +8578,7 @@
         <v>0.1</v>
       </c>
       <c r="I99">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="J99" s="3">
         <v>0</v>
@@ -8594,10 +8594,10 @@
         <v>18</v>
       </c>
       <c r="N99" s="7">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="O99">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="P99" s="3">
         <v>0</v>
@@ -8670,10 +8670,10 @@
         <v>18</v>
       </c>
       <c r="N100" s="7">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="O100">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="P100" s="3">
         <v>0</v>
@@ -8730,7 +8730,7 @@
         <v>0.1</v>
       </c>
       <c r="I101">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J101" s="3">
         <v>0</v>
@@ -8746,10 +8746,10 @@
         <v>18</v>
       </c>
       <c r="N101" s="7">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="O101">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="P101" s="3">
         <v>0</v>
@@ -8806,7 +8806,7 @@
         <v>0.1</v>
       </c>
       <c r="I102">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J102" s="3">
         <v>0</v>
@@ -8822,10 +8822,10 @@
         <v>18</v>
       </c>
       <c r="N102" s="7">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="O102">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="P102" s="3">
         <v>0</v>

</xml_diff>